<commit_message>
Updates for fom and vom costs
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/01_input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/01_input_data/03_overview_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="8_{9BF03DD1-792C-45A1-9F33-181372BB8CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AEBB3A9-866E-4049-8806-4FB7C9E6090D}"/>
+  <xr:revisionPtr revIDLastSave="372" documentId="8_{9BF03DD1-792C-45A1-9F33-181372BB8CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CE0107C-84AC-44A1-9245-98D34C4F01A2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
@@ -290,9 +290,6 @@
     <t>max number invested</t>
   </si>
   <si>
-    <t>potentially take usual yearly value/typical running hours OR time patterns?</t>
-  </si>
-  <si>
     <t>is there an upper limit?</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>Pipeline methanol storage</t>
+  </si>
+  <si>
+    <t>yearly costs / 8760</t>
   </si>
 </sst>
 </file>
@@ -357,15 +357,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -413,18 +410,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:F119" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:F119" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F119" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
     <sortCondition ref="A1:A119"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2ED558C3-764D-4861-A0AF-87ABE40B1777}" name="Type" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{6193EBB5-37EA-4A06-B2F7-25025D1A1AAB}" name="Value" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{ACD2F4FB-0203-4250-BCB2-42328928AC64}" name="Value type" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0699498D-2FCA-46FD-94D0-5795DF694AF9}" name="Comment" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E412C2F9-B9AE-4801-9358-B79EB61E5403}" name="Source" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2ED558C3-764D-4861-A0AF-87ABE40B1777}" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{6193EBB5-37EA-4A06-B2F7-25025D1A1AAB}" name="Value" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{ACD2F4FB-0203-4250-BCB2-42328928AC64}" name="Value type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0699498D-2FCA-46FD-94D0-5795DF694AF9}" name="Comment" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E412C2F9-B9AE-4801-9358-B79EB61E5403}" name="Source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -729,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,7 +797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -811,7 +808,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -825,7 +822,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -886,7 +883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -897,7 +894,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -911,7 +908,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -992,7 +989,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1000,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1017,7 +1014,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1097,7 +1094,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>15</v>
@@ -1108,7 +1105,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>15</v>
@@ -1155,7 +1152,7 @@
         <v>48</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>15</v>
@@ -1166,7 +1163,7 @@
         <v>48</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>15</v>
@@ -1253,7 +1250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>35</v>
       </c>
@@ -1264,7 +1261,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1278,7 +1275,7 @@
         <v>15</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1305,7 +1302,7 @@
     </row>
     <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>51</v>
@@ -1319,7 +1316,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>53</v>
@@ -1333,7 +1330,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>80</v>
@@ -1344,7 +1341,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>81</v>
@@ -1355,7 +1352,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>53</v>
@@ -1369,7 +1366,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>80</v>
@@ -1380,7 +1377,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>81</v>
@@ -1458,11 +1455,11 @@
       <c r="E56" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>32</v>
       </c>
@@ -1470,7 +1467,7 @@
         <v>25</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -1484,7 +1481,7 @@
         <v>15</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -1702,12 +1699,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1847,12 +1844,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data for methanol synthesis
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA41AC92-306B-4D24-BE62-72119D168E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38593634-625D-4091-BDE5-B5A46049C409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="125">
   <si>
     <t>Comment</t>
   </si>
@@ -203,21 +203,12 @@
     <t>power : water</t>
   </si>
   <si>
-    <t>hydrogen : Vap. CO2</t>
-  </si>
-  <si>
     <t>CO2 : Vap. CO2 (+ losses?)</t>
   </si>
   <si>
     <t>raw methanol : e-methanol</t>
   </si>
   <si>
-    <t>hydrogen : raw methanol</t>
-  </si>
-  <si>
-    <t>raw methanol : waste heat</t>
-  </si>
-  <si>
     <t xml:space="preserve">pipeline capacity to/from storage; any losses: fix ratio </t>
   </si>
   <si>
@@ -320,9 +311,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>€ / MW methanol</t>
-  </si>
-  <si>
     <t>Value 2020</t>
   </si>
   <si>
@@ -345,13 +333,99 @@
   </si>
   <si>
     <t>https://ens.dk/sites/ens.dk/files/Analyser/technology_data_for_renewable_fuels.pdf</t>
+  </si>
+  <si>
+    <t>M€ / MW methanol</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>depends on local conditions</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>% of capacity / hour</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0016236121018019</t>
+  </si>
+  <si>
+    <t>24-48</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>for cold start up</t>
+  </si>
+  <si>
+    <t>t / t methanol</t>
+  </si>
+  <si>
+    <t>Mwh / t methanol</t>
+  </si>
+  <si>
+    <t>MWh / MWh total input</t>
+  </si>
+  <si>
+    <t>wee need raw methanol : waste heat</t>
+  </si>
+  <si>
+    <t>we need hydrogen : Vap. CO2  (value is for methanol not the raw methanol)</t>
+  </si>
+  <si>
+    <t>hydrogen : raw methanol  (value is for methanol not the raw methanol)</t>
+  </si>
+  <si>
+    <t>output of water</t>
+  </si>
+  <si>
+    <t>we need electricity : raw methanol  (value is for methanol not the raw methanol)</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>outages per year</t>
+  </si>
+  <si>
+    <t>GJ / t methanol</t>
+  </si>
+  <si>
+    <t>specific energy content</t>
+  </si>
+  <si>
+    <t>Steam / raw methanol (value is for methanol not the raw methanol) + seems to be input for distillation tower</t>
+  </si>
+  <si>
+    <t>k€ / MW methanol</t>
+  </si>
+  <si>
+    <t>start up limit</t>
+  </si>
+  <si>
+    <t>shut down limit</t>
+  </si>
+  <si>
+    <t>lets look of we can use this, e.g., to model longer times to restart after a shut down</t>
+  </si>
+  <si>
+    <t>lets look of we can use this, e.g., to model longer times to restart before a shut down</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0_)"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,16 +455,99 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Helv"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -398,9 +555,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="63"/>
+      </left>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top style="thin">
+        <color indexed="63"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="62"/>
+      </top>
+      <bottom style="double">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -413,8 +644,38 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="31">
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{CA87A11B-7565-4B80-9ACA-4E9D38A9573D}"/>
+    <cellStyle name="Comma 2 2" xfId="8" xr:uid="{3FE2516D-5C90-4C04-B8CD-F3AECD71F538}"/>
+    <cellStyle name="Comma 3" xfId="9" xr:uid="{04636A24-A7D9-404D-A03D-AE71DC5E8E6A}"/>
+    <cellStyle name="Comma 4" xfId="1" xr:uid="{6E627487-B94E-4A2C-A346-AB0CDCBBA86C}"/>
+    <cellStyle name="Comma0 - Type3" xfId="10" xr:uid="{D2647E7A-CA20-4068-8BA8-0132F12085EE}"/>
+    <cellStyle name="Fixed2 - Type2" xfId="11" xr:uid="{D8410020-C2BC-4987-870A-2342F851D304}"/>
+    <cellStyle name="Hyperlink 2" xfId="12" xr:uid="{F87AABDB-ADB7-4C25-B5CC-EE2729DE4045}"/>
+    <cellStyle name="Hyperlink 3" xfId="13" xr:uid="{BD5DBDF0-273A-4E1B-91C7-420FB7565EA6}"/>
+    <cellStyle name="Input 2" xfId="14" xr:uid="{AFC1BFE4-0B17-407B-AC1B-F41A2651C770}"/>
+    <cellStyle name="Input 2 2" xfId="26" xr:uid="{365509C8-9741-4ED5-BFBD-F161ABBC53CB}"/>
+    <cellStyle name="Komma 2" xfId="15" xr:uid="{CF4C032B-C635-445F-9FF6-0F5F49C11B69}"/>
+    <cellStyle name="Komma 3" xfId="16" xr:uid="{552A0DD5-1944-4DF8-A758-45847BA2DC25}"/>
+    <cellStyle name="Link 2" xfId="4" xr:uid="{22B1E4C3-E0F5-4829-B956-FF18563948C5}"/>
+    <cellStyle name="Neutral 2" xfId="17" xr:uid="{9830AF80-8B52-43E3-B37B-202E95A097B5}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="2" xr:uid="{29527CFF-E131-4C85-B1F4-446CC779502C}"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{75A81AB8-43BA-42B1-9BFE-3442D08D323D}"/>
+    <cellStyle name="Normal 2 2" xfId="18" xr:uid="{A487AA04-3645-48E2-BF05-D102C92D741A}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{7E4BC29C-7874-4571-84F5-4A1AD8C4340C}"/>
+    <cellStyle name="Normal 4" xfId="29" xr:uid="{320AAF4C-5EE7-485E-8091-D4E38B56F58B}"/>
+    <cellStyle name="Normal 6" xfId="19" xr:uid="{DCE4CC68-0454-4C22-BBD2-7812694A1005}"/>
+    <cellStyle name="Normal 6 2" xfId="20" xr:uid="{B77E1514-5F2D-4335-B5CC-96A0E99D4FD6}"/>
+    <cellStyle name="Output 2" xfId="21" xr:uid="{4A556491-6ADD-49B5-8F72-DF8D0A5BB713}"/>
+    <cellStyle name="Output 2 2" xfId="27" xr:uid="{CD5E1D33-74BF-49F0-887B-A29C72391095}"/>
+    <cellStyle name="Percen - Type1" xfId="22" xr:uid="{D301B74E-DDA6-432D-A768-4ADA0D35B784}"/>
+    <cellStyle name="Percent 2" xfId="7" xr:uid="{4133C472-81D1-488D-85DA-D2156BB51092}"/>
+    <cellStyle name="Percent 3" xfId="30" xr:uid="{835FA606-D757-4ED2-AAAB-7C9DD597D990}"/>
+    <cellStyle name="Procent 2" xfId="23" xr:uid="{7CDBB6E3-1A76-4178-A1A4-CA867E8C9B97}"/>
+    <cellStyle name="Procent 3" xfId="24" xr:uid="{DA978252-2B8A-4B3F-8897-D27AE9E9D6C1}"/>
+    <cellStyle name="Total 2" xfId="25" xr:uid="{494D1728-9EE3-4E03-932D-5565C69D7F26}"/>
+    <cellStyle name="Total 2 2" xfId="28" xr:uid="{08E68298-B52F-4B3E-8C41-DE0BEBA47065}"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -470,23 +731,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K119" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K119" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K66">
-    <sortCondition ref="A1:A119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K129" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K129" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K76">
+    <sortCondition ref="A1:A129"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{2ED558C3-764D-4861-A0AF-87ABE40B1777}" name="Type" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{6193EBB5-37EA-4A06-B2F7-25025D1A1AAB}" name="Value 2020" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{739A6CD2-FFD4-4D7F-A624-B09406414C1C}" name="Value 2025" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{E9026FFC-D629-4035-9CCD-90E73F77B645}" name="Value 2030" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{FCB3F86B-32A8-4B41-9D9C-301567A77ADF}" name="Value 2040" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{E973AC09-1E45-4115-BB46-B8ABA81C6463}" name="Value 2050" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{BE5EBBB4-C484-47E5-A7E8-D08AF713C5F6}" name="Unit" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{ACD2F4FB-0203-4250-BCB2-42328928AC64}" name="Value type" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{0699498D-2FCA-46FD-94D0-5795DF694AF9}" name="Comment" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{E412C2F9-B9AE-4801-9358-B79EB61E5403}" name="Source" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{739A6CD2-FFD4-4D7F-A624-B09406414C1C}" name="Value 2025" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{E9026FFC-D629-4035-9CCD-90E73F77B645}" name="Value 2030" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{FCB3F86B-32A8-4B41-9D9C-301567A77ADF}" name="Value 2040" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{E973AC09-1E45-4115-BB46-B8ABA81C6463}" name="Value 2050" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{BE5EBBB4-C484-47E5-A7E8-D08AF713C5F6}" name="Unit" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{ACD2F4FB-0203-4250-BCB2-42328928AC64}" name="Value type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0699498D-2FCA-46FD-94D0-5795DF694AF9}" name="Comment" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E412C2F9-B9AE-4801-9358-B79EB61E5403}" name="Source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -789,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -815,22 +1076,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>13</v>
@@ -864,7 +1125,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -889,7 +1150,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -897,13 +1158,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -911,7 +1172,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>14</v>
@@ -950,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -975,7 +1236,7 @@
         <v>14</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -983,13 +1244,13 @@
         <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -997,7 +1258,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>14</v>
@@ -1025,7 +1286,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>23</v>
@@ -1042,7 +1303,7 @@
         <v>14</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1067,7 +1328,7 @@
         <v>11</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1081,7 +1342,7 @@
         <v>14</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1089,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -1103,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>14</v>
@@ -1139,7 +1400,7 @@
         <v>41</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -1161,13 +1422,13 @@
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -1175,7 +1436,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>14</v>
@@ -1186,7 +1447,7 @@
         <v>46</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>14</v>
@@ -1194,7 +1455,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>12</v>
@@ -1205,13 +1466,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -1219,13 +1480,13 @@
         <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -1233,7 +1494,7 @@
         <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>14</v>
@@ -1244,18 +1505,36 @@
         <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>14</v>
@@ -1272,22 +1551,22 @@
         <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>14</v>
@@ -1296,352 +1575,631 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="C37" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="I37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="C38" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="E38" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="F38" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="G38" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="I38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="C39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="I39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J40" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C41" s="3">
-        <v>39</v>
+        <v>0.1</v>
       </c>
       <c r="D41" s="3">
-        <v>39</v>
+        <v>0.1</v>
       </c>
       <c r="E41" s="3">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="F41" s="3">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="G41" s="3">
-        <v>26</v>
+        <v>0.1</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C42" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D42" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E42" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F42" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G42" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K43" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="3">
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>39</v>
+      </c>
+      <c r="E44" s="3">
+        <v>30</v>
+      </c>
+      <c r="F44" s="3">
+        <v>30</v>
+      </c>
+      <c r="G44" s="3">
+        <v>26</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I44" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>79</v>
+      <c r="C47" s="3">
+        <v>30</v>
+      </c>
+      <c r="D47" s="3">
+        <v>30</v>
+      </c>
+      <c r="E47" s="3">
+        <v>30</v>
+      </c>
+      <c r="F47" s="3">
+        <v>30</v>
+      </c>
+      <c r="G47" s="3">
+        <v>30</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>79</v>
+      <c r="C50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="C53" s="3">
+        <v>3</v>
+      </c>
+      <c r="D53" s="3">
+        <v>3</v>
+      </c>
+      <c r="E53" s="3">
+        <v>3</v>
+      </c>
+      <c r="F53" s="3">
+        <v>3</v>
+      </c>
+      <c r="G53" s="3">
+        <v>3</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+      <c r="C54" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="D54" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E54" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F54" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G54" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>65</v>
+        <v>118</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="J55" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>14</v>
@@ -1649,10 +2207,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>14</v>
@@ -1660,7 +2218,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>50</v>
@@ -1669,50 +2227,181 @@
         <v>14</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B72" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="I73" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J64" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+      <c r="J74" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J65" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" s="3" t="s">
+      <c r="J75" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I66" s="3" t="s">
+      <c r="I76" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1741,7 +2430,7 @@
           <x14:formula1>
             <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>H120:H1048576 I1:I119</xm:sqref>
+          <xm:sqref>H130:H1048576 I1:I129</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1796,7 +2485,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
@@ -1836,17 +2525,17 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1856,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A04CB00-B233-4C8F-9598-9E4FA54AC391}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1956,57 +2645,67 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data need structure for electrolysis
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38593634-625D-4091-BDE5-B5A46049C409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F98860E-CDEA-4A64-8CB3-5C1448832351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="130">
   <si>
     <t>Comment</t>
   </si>
@@ -251,9 +251,6 @@
     <t>variable? Fix?</t>
   </si>
   <si>
-    <t>capactiy waste_heat</t>
-  </si>
-  <si>
     <t>capacity hydrogen</t>
   </si>
   <si>
@@ -414,6 +411,24 @@
   </si>
   <si>
     <t>lets look of we can use this, e.g., to model longer times to restart before a shut down</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>€ / MWh hydrogen</t>
+  </si>
+  <si>
+    <t>Electrolyzer AEC</t>
+  </si>
+  <si>
+    <t>Electrolyzer SOEC</t>
+  </si>
+  <si>
+    <t>Electrolyzer PEM</t>
+  </si>
+  <si>
+    <t>€ / kW</t>
   </si>
 </sst>
 </file>
@@ -422,8 +437,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0_)"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0_)"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -599,15 +614,15 @@
   </borders>
   <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -617,7 +632,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -731,10 +746,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K129" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K129" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K76">
-    <sortCondition ref="A1:A129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K130" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K130" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K77">
+    <sortCondition ref="A1:A130"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="10"/>
@@ -1050,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,22 +1091,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>13</v>
@@ -1150,7 +1165,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1158,13 +1173,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1172,7 +1187,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>14</v>
@@ -1236,7 +1251,7 @@
         <v>14</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1244,13 +1259,13 @@
         <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1258,7 +1273,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>14</v>
@@ -1286,27 +1301,45 @@
         <v>19</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="I17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -1320,173 +1353,260 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>77</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3">
+        <v>550</v>
+      </c>
+      <c r="G21" s="3">
+        <v>300</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="3">
+        <v>650</v>
+      </c>
+      <c r="G22" s="3">
+        <v>350</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="3">
+        <v>775</v>
+      </c>
+      <c r="G23" s="3">
+        <v>500</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="I24" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="C26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J28" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -1494,10 +1614,13 @@
         <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -1505,45 +1628,24 @@
         <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1551,63 +1653,60 @@
         <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D37" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="E37" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="G37" s="3">
-        <v>1.4</v>
+        <v>11</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1618,31 +1717,31 @@
         <v>52</v>
       </c>
       <c r="C38" s="3">
-        <v>6.4</v>
+        <v>1.4</v>
       </c>
       <c r="D38" s="3">
-        <v>6.4</v>
+        <v>1.4</v>
       </c>
       <c r="E38" s="3">
-        <v>6.4</v>
+        <v>1.4</v>
       </c>
       <c r="F38" s="3">
-        <v>6.4</v>
+        <v>1.4</v>
       </c>
       <c r="G38" s="3">
-        <v>6.4</v>
+        <v>1.4</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1653,31 +1752,31 @@
         <v>52</v>
       </c>
       <c r="C39" s="3">
-        <v>0.2</v>
+        <v>6.4</v>
       </c>
       <c r="D39" s="3">
-        <v>0.2</v>
+        <v>6.4</v>
       </c>
       <c r="E39" s="3">
-        <v>0.2</v>
+        <v>6.4</v>
       </c>
       <c r="F39" s="3">
-        <v>0.2</v>
+        <v>6.4</v>
       </c>
       <c r="G39" s="3">
-        <v>0.2</v>
+        <v>6.4</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1688,31 +1787,31 @@
         <v>52</v>
       </c>
       <c r="C40" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="D40" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="E40" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="F40" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="G40" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1723,31 +1822,31 @@
         <v>52</v>
       </c>
       <c r="C41" s="3">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D41" s="3">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E41" s="3">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F41" s="3">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G41" s="3">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1758,31 +1857,31 @@
         <v>52</v>
       </c>
       <c r="C42" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="D42" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="E42" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="F42" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="G42" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1790,31 +1889,34 @@
         <v>34</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C43" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D43" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E43" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F43" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G43" s="3">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="J43" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="K43" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1822,95 +1924,95 @@
         <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C44" s="3">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D44" s="3">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E44" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F44" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G44" s="3">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J44" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="K44" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>100</v>
+        <v>24</v>
+      </c>
+      <c r="C45" s="3">
+        <v>39</v>
+      </c>
+      <c r="D45" s="3">
+        <v>39</v>
+      </c>
+      <c r="E45" s="3">
+        <v>30</v>
+      </c>
+      <c r="F45" s="3">
+        <v>30</v>
+      </c>
+      <c r="G45" s="3">
+        <v>26</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="3">
-        <v>1.35</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1.35</v>
-      </c>
-      <c r="E46" s="3">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0.87</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>97</v>
+      <c r="J46" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1918,63 +2020,63 @@
         <v>34</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C47" s="3">
-        <v>30</v>
+        <v>1.35</v>
       </c>
       <c r="D47" s="3">
-        <v>30</v>
+        <v>1.35</v>
       </c>
       <c r="E47" s="3">
-        <v>30</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F47" s="3">
-        <v>30</v>
+        <v>0.96</v>
       </c>
       <c r="G47" s="3">
-        <v>30</v>
+        <v>0.87</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="C48" s="3">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="D48" s="3">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="E48" s="3">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="F48" s="3">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="G48" s="3">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1982,7 +2084,7 @@
         <v>34</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C49" s="3">
         <v>0.5</v>
@@ -2000,13 +2102,13 @@
         <v>0.5</v>
       </c>
       <c r="H49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -2014,48 +2116,66 @@
         <v>34</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>104</v>
+        <v>86</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.5</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>121</v>
+        <v>84</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>123</v>
+        <v>105</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
@@ -2063,42 +2183,27 @@
         <v>34</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="3">
-        <v>3</v>
-      </c>
-      <c r="D53" s="3">
-        <v>3</v>
-      </c>
-      <c r="E53" s="3">
-        <v>3</v>
-      </c>
-      <c r="F53" s="3">
-        <v>3</v>
-      </c>
-      <c r="G53" s="3">
-        <v>3</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>115</v>
+      <c r="B53" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -2106,75 +2211,93 @@
         <v>34</v>
       </c>
       <c r="C54" s="3">
+        <v>3</v>
+      </c>
+      <c r="D54" s="3">
+        <v>3</v>
+      </c>
+      <c r="E54" s="3">
+        <v>3</v>
+      </c>
+      <c r="F54" s="3">
+        <v>3</v>
+      </c>
+      <c r="G54" s="3">
+        <v>3</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D55" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E55" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F55" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G55" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J55" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J54" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>56</v>
+      <c r="K55" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>14</v>
@@ -2182,35 +2305,35 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>14</v>
@@ -2218,16 +2341,13 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
@@ -2235,69 +2355,72 @@
         <v>36</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I65" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J64" s="3" t="s">
+      <c r="J65" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K64" s="4" t="s">
+      <c r="K65" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>84</v>
+        <v>59</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
@@ -2305,13 +2428,10 @@
         <v>31</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
@@ -2319,10 +2439,13 @@
         <v>31</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
@@ -2330,7 +2453,7 @@
         <v>31</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>14</v>
@@ -2338,10 +2461,10 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>14</v>
@@ -2349,16 +2472,13 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
@@ -2366,10 +2486,13 @@
         <v>35</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
@@ -2377,10 +2500,10 @@
         <v>35</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>67</v>
+        <v>43</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
@@ -2388,20 +2511,31 @@
         <v>35</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I76" s="3" t="s">
+      <c r="I77" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2414,6 +2548,12 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{367FBE37-4BB4-4A2D-B61E-D7A013871256}">
+          <x14:formula1>
+            <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>H131:H1048576 I1:I130</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7911B029-FECC-467E-9742-40BD9EB9AF02}">
           <x14:formula1>
             <xm:f>Variables!$A$2:$A$51</xm:f>
@@ -2422,15 +2562,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DCFF093-BE81-4C53-B36B-4DFE1729FE77}">
           <x14:formula1>
-            <xm:f>Objects!$A$3:$A$86</xm:f>
+            <xm:f>Objects!$A$3:$A$89</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{367FBE37-4BB4-4A2D-B61E-D7A013871256}">
-          <x14:formula1>
-            <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
-          </x14:formula1>
-          <xm:sqref>H130:H1048576 I1:I129</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2440,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B686478B-2667-46C0-A34E-67E3B0146B50}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2465,77 +2599,92 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2650,62 +2799,62 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a missing parameter description
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1540CFF-C354-4C84-88FF-879A0D94F7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B0C75-3179-407E-92AF-90124A17ABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="144">
   <si>
     <t>Comment</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>days per year</t>
+  </si>
+  <si>
+    <t>use default model value</t>
   </si>
 </sst>
 </file>
@@ -785,10 +788,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K156" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K156" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K103">
-    <sortCondition ref="A1:A156"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K159" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K159" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K106">
+    <sortCondition ref="A1:A159"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="10"/>
@@ -1104,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2525,13 +2528,31 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="I53" s="3" t="s">
         <v>14</v>
       </c>
@@ -2539,12 +2560,30 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>63</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>14</v>
@@ -2577,46 +2616,25 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>14</v>
@@ -2624,182 +2642,113 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C64" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D64" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="E64" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="F64" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="G64" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="I64" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J64" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C65" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="D65" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="E65" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="F65" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="G65" s="3">
-        <v>6.4</v>
+        <v>11</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C66" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D66" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E66" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F66" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G66" s="3">
-        <v>0.2</v>
+        <v>11</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="K66" s="3" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -2810,19 +2759,19 @@
         <v>52</v>
       </c>
       <c r="C67" s="3">
-        <v>0.55000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="D67" s="3">
-        <v>0.55000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="E67" s="3">
-        <v>0.55000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="F67" s="3">
-        <v>0.55000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="G67" s="3">
-        <v>0.55000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>106</v>
@@ -2831,7 +2780,7 @@
         <v>14</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K67" s="3" t="s">
         <v>96</v>
@@ -2845,19 +2794,19 @@
         <v>52</v>
       </c>
       <c r="C68" s="3">
-        <v>0.1</v>
+        <v>6.4</v>
       </c>
       <c r="D68" s="3">
-        <v>0.1</v>
+        <v>6.4</v>
       </c>
       <c r="E68" s="3">
-        <v>0.1</v>
+        <v>6.4</v>
       </c>
       <c r="F68" s="3">
-        <v>0.1</v>
+        <v>6.4</v>
       </c>
       <c r="G68" s="3">
-        <v>0.1</v>
+        <v>6.4</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>107</v>
@@ -2866,7 +2815,7 @@
         <v>14</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K68" s="3" t="s">
         <v>96</v>
@@ -2880,28 +2829,28 @@
         <v>52</v>
       </c>
       <c r="C69" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="D69" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="E69" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="F69" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="G69" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>96</v>
@@ -2912,28 +2861,31 @@
         <v>34</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C70" s="3">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D70" s="3">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E70" s="3">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F70" s="3">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G70" s="3">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>96</v>
@@ -2944,63 +2896,69 @@
         <v>34</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C71" s="3">
-        <v>39</v>
+        <v>0.1</v>
       </c>
       <c r="D71" s="3">
-        <v>39</v>
+        <v>0.1</v>
       </c>
       <c r="E71" s="3">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="F71" s="3">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="G71" s="3">
-        <v>26</v>
+        <v>0.1</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>99</v>
+        <v>52</v>
+      </c>
+      <c r="C72" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F72" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G72" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>78</v>
+        <v>118</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3008,25 +2966,25 @@
         <v>34</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="C73" s="3">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="D73" s="3">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E73" s="3">
-        <v>1.0900000000000001</v>
+        <v>0</v>
       </c>
       <c r="F73" s="3">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="G73" s="3">
-        <v>0.87</v>
+        <v>0</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>14</v>
@@ -3040,13 +2998,13 @@
         <v>34</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C74" s="3">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D74" s="3">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E74" s="3">
         <v>30</v>
@@ -3055,48 +3013,48 @@
         <v>30</v>
       </c>
       <c r="G74" s="3">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="J74" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="K74" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C75" s="3">
-        <v>50</v>
-      </c>
-      <c r="D75" s="3">
-        <v>50</v>
-      </c>
-      <c r="E75" s="3">
-        <v>50</v>
-      </c>
-      <c r="F75" s="3">
-        <v>50</v>
-      </c>
-      <c r="G75" s="3">
-        <v>50</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>101</v>
+        <v>77</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K75" s="3" t="s">
-        <v>102</v>
+      <c r="J75" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3104,31 +3062,31 @@
         <v>34</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C76" s="3">
-        <v>50</v>
+        <v>1.35</v>
       </c>
       <c r="D76" s="3">
-        <v>50</v>
+        <v>1.35</v>
       </c>
       <c r="E76" s="3">
-        <v>50</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F76" s="3">
-        <v>50</v>
+        <v>0.96</v>
       </c>
       <c r="G76" s="3">
-        <v>50</v>
+        <v>0.87</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3136,159 +3094,219 @@
         <v>34</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>103</v>
+        <v>28</v>
+      </c>
+      <c r="C77" s="3">
+        <v>30</v>
+      </c>
+      <c r="D77" s="3">
+        <v>30</v>
+      </c>
+      <c r="E77" s="3">
+        <v>30</v>
+      </c>
+      <c r="F77" s="3">
+        <v>30</v>
+      </c>
+      <c r="G77" s="3">
+        <v>30</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>120</v>
+        <v>85</v>
+      </c>
+      <c r="C78" s="3">
+        <v>50</v>
+      </c>
+      <c r="D78" s="3">
+        <v>50</v>
+      </c>
+      <c r="E78" s="3">
+        <v>50</v>
+      </c>
+      <c r="F78" s="3">
+        <v>50</v>
+      </c>
+      <c r="G78" s="3">
+        <v>50</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J78" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K78" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>121</v>
+        <v>86</v>
+      </c>
+      <c r="C79" s="3">
+        <v>50</v>
+      </c>
+      <c r="D79" s="3">
+        <v>50</v>
+      </c>
+      <c r="E79" s="3">
+        <v>50</v>
+      </c>
+      <c r="F79" s="3">
+        <v>50</v>
+      </c>
+      <c r="G79" s="3">
+        <v>50</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J79" s="3" t="s">
-        <v>123</v>
+      <c r="K79" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C80" s="3">
-        <v>3</v>
-      </c>
-      <c r="D80" s="3">
-        <v>3</v>
-      </c>
-      <c r="E80" s="3">
-        <v>3</v>
-      </c>
-      <c r="F80" s="3">
-        <v>3</v>
-      </c>
-      <c r="G80" s="3">
-        <v>3</v>
+      <c r="B80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C81" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="D81" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="E81" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="F81" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G81" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>116</v>
+      <c r="B81" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="I82" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>14</v>
+        <v>141</v>
+      </c>
+      <c r="C83" s="3">
+        <v>3</v>
+      </c>
+      <c r="D83" s="3">
+        <v>3</v>
+      </c>
+      <c r="E83" s="3">
+        <v>3</v>
+      </c>
+      <c r="F83" s="3">
+        <v>3</v>
+      </c>
+      <c r="G83" s="3">
+        <v>3</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="C84" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="D84" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E84" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F84" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G84" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
@@ -3296,15 +3314,18 @@
         <v>81</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="I85" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>52</v>
@@ -3318,7 +3339,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>75</v>
@@ -3329,7 +3350,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>76</v>
@@ -3340,86 +3361,83 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="I90" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J90" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J91" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K91" s="4" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="J92" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I93" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I94" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J93" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K93" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J94" s="3" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
@@ -3427,24 +3445,27 @@
         <v>31</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="I95" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J95" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
@@ -3452,57 +3473,57 @@
         <v>31</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I97" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="I98" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J101" s="3" t="s">
-        <v>67</v>
+      <c r="I101" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
@@ -3510,20 +3531,56 @@
         <v>35</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I103" s="3" t="s">
+      <c r="I106" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3540,7 +3597,7 @@
           <x14:formula1>
             <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>H157:H1048576 I1:I156</xm:sqref>
+          <xm:sqref>H160:H1048576 I1:I159</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DCFF093-BE81-4C53-B36B-4DFE1729FE77}">
           <x14:formula1>

</xml_diff>

<commit_message>
add parameters for hydrogen storage
next step is adding the values
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B0C75-3179-407E-92AF-90124A17ABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B19C619-FC51-4C4C-BA17-E624C93A185C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="148">
   <si>
     <t>Comment</t>
   </si>
@@ -471,6 +471,18 @@
   </si>
   <si>
     <t>use default model value</t>
+  </si>
+  <si>
+    <t>efficiency for charging</t>
+  </si>
+  <si>
+    <t>efficiency for discharging</t>
+  </si>
+  <si>
+    <t>loss rate during the given period</t>
+  </si>
+  <si>
+    <t>input capacity of the storage, might depend on the storage capacity, TBA</t>
   </si>
 </sst>
 </file>
@@ -788,10 +800,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K159" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K159" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K106">
-    <sortCondition ref="A1:A159"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K163" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K163" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K110">
+    <sortCondition ref="A1:A163"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="10"/>
@@ -1107,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2596,11 +2608,11 @@
       <c r="A55" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="I55" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -2608,7 +2620,7 @@
         <v>46</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>14</v>
@@ -2618,59 +2630,80 @@
       <c r="A57" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="B57" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="I58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="B59" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>69</v>
+        <v>24</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>14</v>
@@ -2678,217 +2711,124 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B66" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I64" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C67" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D67" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="E67" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="F67" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="G67" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C68" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="D68" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="E68" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="F68" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="G68" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="I68" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J68" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C69" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D69" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E69" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F69" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G69" s="3">
-        <v>0.2</v>
+        <v>11</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C70" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D70" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E70" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F70" s="3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G70" s="3">
-        <v>0.55000000000000004</v>
+        <v>11</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -2899,28 +2839,28 @@
         <v>52</v>
       </c>
       <c r="C71" s="3">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="D71" s="3">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="E71" s="3">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="F71" s="3">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="G71" s="3">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>96</v>
@@ -2934,19 +2874,19 @@
         <v>52</v>
       </c>
       <c r="C72" s="3">
-        <v>0.57999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="D72" s="3">
-        <v>0.57999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="E72" s="3">
-        <v>0.57999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="F72" s="3">
-        <v>0.57999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="G72" s="3">
-        <v>0.57999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>107</v>
@@ -2955,7 +2895,7 @@
         <v>14</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>96</v>
@@ -2966,28 +2906,31 @@
         <v>34</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C73" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D73" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E73" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F73" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G73" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>96</v>
@@ -2998,63 +2941,69 @@
         <v>34</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C74" s="3">
-        <v>39</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D74" s="3">
-        <v>39</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E74" s="3">
-        <v>30</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F74" s="3">
-        <v>30</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G74" s="3">
-        <v>26</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>99</v>
+        <v>52</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F75" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G75" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>78</v>
+        <v>113</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3062,28 +3011,31 @@
         <v>34</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C76" s="3">
-        <v>1.35</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D76" s="3">
-        <v>1.35</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E76" s="3">
-        <v>1.0900000000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F76" s="3">
-        <v>0.96</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G76" s="3">
-        <v>0.87</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="K76" s="3" t="s">
         <v>96</v>
@@ -3094,25 +3046,25 @@
         <v>34</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C77" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D77" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E77" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F77" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G77" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I77" s="3" t="s">
         <v>14</v>
@@ -3126,63 +3078,63 @@
         <v>34</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="C78" s="3">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D78" s="3">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E78" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F78" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G78" s="3">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="J78" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="K78" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C79" s="3">
-        <v>50</v>
-      </c>
-      <c r="D79" s="3">
-        <v>50</v>
-      </c>
-      <c r="E79" s="3">
-        <v>50</v>
-      </c>
-      <c r="F79" s="3">
-        <v>50</v>
-      </c>
-      <c r="G79" s="3">
-        <v>50</v>
-      </c>
-      <c r="H79" s="3" t="s">
-        <v>101</v>
+        <v>77</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K79" s="3" t="s">
-        <v>102</v>
+      <c r="J79" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3190,62 +3142,95 @@
         <v>34</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>103</v>
+        <v>74</v>
+      </c>
+      <c r="C80" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="D80" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="E80" s="3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F80" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="G80" s="3">
+        <v>0.87</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>120</v>
+        <v>28</v>
+      </c>
+      <c r="C81" s="3">
+        <v>30</v>
+      </c>
+      <c r="D81" s="3">
+        <v>30</v>
+      </c>
+      <c r="E81" s="3">
+        <v>30</v>
+      </c>
+      <c r="F81" s="3">
+        <v>30</v>
+      </c>
+      <c r="G81" s="3">
+        <v>30</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J81" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K81" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>121</v>
+        <v>85</v>
+      </c>
+      <c r="C82" s="3">
+        <v>50</v>
+      </c>
+      <c r="D82" s="3">
+        <v>50</v>
+      </c>
+      <c r="E82" s="3">
+        <v>50</v>
+      </c>
+      <c r="F82" s="3">
+        <v>50</v>
+      </c>
+      <c r="G82" s="3">
+        <v>50</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="I82" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J82" s="3" t="s">
-        <v>123</v>
+      <c r="K82" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3253,57 +3238,63 @@
         <v>34</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
       <c r="C83" s="3">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D83" s="3">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E83" s="3">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="F83" s="3">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="G83" s="3">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>115</v>
+        <v>101</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C84" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="D84" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="E84" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="F84" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G84" s="3">
-        <v>19.899999999999999</v>
+      <c r="B84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="K84" s="3" t="s">
         <v>96</v>
@@ -3311,85 +3302,127 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="I85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="I86" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+      <c r="C87" s="3">
+        <v>3</v>
+      </c>
+      <c r="D87" s="3">
+        <v>3</v>
+      </c>
+      <c r="E87" s="3">
+        <v>3</v>
+      </c>
+      <c r="F87" s="3">
+        <v>3</v>
+      </c>
+      <c r="G87" s="3">
+        <v>3</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="C88" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="D88" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E88" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F88" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G88" s="3">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="I90" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I91" s="3" t="s">
         <v>14</v>
@@ -3397,21 +3430,18 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J92" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>52</v>
@@ -3423,164 +3453,214 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J94" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K94" s="4" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="I95" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="I96" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I98" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J96" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J97" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="J98" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I100" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A101" s="3" t="s">
+      <c r="I104" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I101" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+      <c r="I105" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I102" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J102" s="3" t="s">
+      <c r="I106" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J106" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="s">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I103" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="s">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J104" s="3" t="s">
+      <c r="J108" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A105" s="3" t="s">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J105" s="3" t="s">
+      <c r="J109" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A106" s="3" t="s">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="I110" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3597,7 +3677,7 @@
           <x14:formula1>
             <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>H160:H1048576 I1:I159</xm:sqref>
+          <xm:sqref>H164:H1048576 I1:I163</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DCFF093-BE81-4C53-B36B-4DFE1729FE77}">
           <x14:formula1>
@@ -3741,7 +3821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A04CB00-B233-4C8F-9598-9E4FA54AC391}">
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding electric steam boiler information
add the information to the raw input data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9298DE1D-75B8-4ED5-936A-00AD5F5F5E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB85277-6435-4375-86BD-BFBE4CCFC7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="251">
   <si>
     <t>Comment</t>
   </si>
@@ -774,6 +774,24 @@
   </si>
   <si>
     <t>1% per day, results in 0,04147% per hour</t>
+  </si>
+  <si>
+    <t>Electric_Steam_Boiler</t>
+  </si>
+  <si>
+    <t>Power/Steam</t>
+  </si>
+  <si>
+    <t>Energy efficiency</t>
+  </si>
+  <si>
+    <t>% of a year</t>
+  </si>
+  <si>
+    <t>[€/MW/year]</t>
+  </si>
+  <si>
+    <t>[M€ per MW]</t>
   </si>
 </sst>
 </file>
@@ -1124,17 +1142,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K186" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K186" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Hydrogen storage"/>
-        <filter val="Methanol storage"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K185" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K185" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K147">
-    <sortCondition ref="A1:A186"/>
+    <sortCondition ref="A1:A185"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="10"/>
@@ -1450,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
-  <dimension ref="A1:K186"/>
+  <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I54" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="H159" sqref="H159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1503,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1543,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1564,7 +1575,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="174" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -1599,7 +1610,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -1625,7 +1636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1654,7 +1665,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1683,7 +1694,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1709,7 +1720,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1720,7 +1731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -1746,7 +1757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -1775,7 +1786,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1801,7 +1812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1830,7 +1841,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1870,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1890,7 +1901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1916,7 +1927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -1933,7 +1944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -1965,7 +1976,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -1994,7 +2005,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
@@ -2026,7 +2037,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>121</v>
       </c>
@@ -2058,7 +2069,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>121</v>
       </c>
@@ -2093,7 +2104,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>121</v>
       </c>
@@ -2128,7 +2139,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>121</v>
       </c>
@@ -2160,7 +2171,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>121</v>
       </c>
@@ -2192,7 +2203,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>121</v>
       </c>
@@ -2227,7 +2238,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>121</v>
       </c>
@@ -2259,7 +2270,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>121</v>
       </c>
@@ -2291,7 +2302,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>121</v>
       </c>
@@ -2323,7 +2334,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>121</v>
       </c>
@@ -2355,7 +2366,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>123</v>
       </c>
@@ -2387,7 +2398,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>123</v>
       </c>
@@ -2422,7 +2433,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>123</v>
       </c>
@@ -2457,7 +2468,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>123</v>
       </c>
@@ -2489,7 +2500,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>123</v>
       </c>
@@ -2521,7 +2532,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>123</v>
       </c>
@@ -2556,7 +2567,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
@@ -2588,7 +2599,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>123</v>
       </c>
@@ -2620,7 +2631,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>123</v>
       </c>
@@ -2652,7 +2663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>123</v>
       </c>
@@ -2684,7 +2695,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>122</v>
       </c>
@@ -2719,7 +2730,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>122</v>
       </c>
@@ -2754,7 +2765,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>122</v>
       </c>
@@ -2786,7 +2797,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>122</v>
       </c>
@@ -2821,7 +2832,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>122</v>
       </c>
@@ -2856,7 +2867,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>122</v>
       </c>
@@ -2888,7 +2899,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>122</v>
       </c>
@@ -2923,7 +2934,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>122</v>
       </c>
@@ -2955,7 +2966,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>122</v>
       </c>
@@ -2987,7 +2998,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>122</v>
       </c>
@@ -3019,7 +3030,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>122</v>
       </c>
@@ -3051,7 +3062,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>40</v>
       </c>
@@ -3080,7 +3091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>40</v>
       </c>
@@ -3298,7 +3309,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
@@ -3309,7 +3320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>56</v>
       </c>
@@ -3364,7 +3375,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>34</v>
       </c>
@@ -3396,7 +3407,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>34</v>
       </c>
@@ -3428,7 +3439,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>34</v>
       </c>
@@ -3463,7 +3474,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>34</v>
       </c>
@@ -3498,7 +3509,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>34</v>
       </c>
@@ -3533,7 +3544,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>34</v>
       </c>
@@ -3568,7 +3579,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>34</v>
       </c>
@@ -3603,7 +3614,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>34</v>
       </c>
@@ -3638,7 +3649,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>34</v>
       </c>
@@ -3670,7 +3681,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>34</v>
       </c>
@@ -3705,7 +3716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>34</v>
       </c>
@@ -3734,7 +3745,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>34</v>
       </c>
@@ -3766,7 +3777,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>34</v>
       </c>
@@ -3798,7 +3809,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>34</v>
       </c>
@@ -3830,7 +3841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>34</v>
       </c>
@@ -3862,7 +3873,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>34</v>
       </c>
@@ -3897,7 +3908,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>34</v>
       </c>
@@ -3911,7 +3922,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>34</v>
       </c>
@@ -3925,7 +3936,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>34</v>
       </c>
@@ -3957,7 +3968,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>34</v>
       </c>
@@ -3986,7 +3997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>183</v>
       </c>
@@ -4012,7 +4023,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>183</v>
       </c>
@@ -4038,7 +4049,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>183</v>
       </c>
@@ -4067,7 +4078,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>183</v>
       </c>
@@ -4096,7 +4107,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>183</v>
       </c>
@@ -4125,7 +4136,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>183</v>
       </c>
@@ -4154,7 +4165,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>183</v>
       </c>
@@ -4183,7 +4194,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>183</v>
       </c>
@@ -4212,7 +4223,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>183</v>
       </c>
@@ -4241,7 +4252,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>183</v>
       </c>
@@ -4270,7 +4281,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>183</v>
       </c>
@@ -4296,7 +4307,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>183</v>
       </c>
@@ -4322,7 +4333,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>79</v>
       </c>
@@ -4351,7 +4362,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>79</v>
       </c>
@@ -4365,7 +4376,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>79</v>
       </c>
@@ -4394,7 +4405,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>79</v>
       </c>
@@ -4423,7 +4434,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>79</v>
       </c>
@@ -4452,7 +4463,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>79</v>
       </c>
@@ -4481,7 +4492,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>79</v>
       </c>
@@ -4510,7 +4521,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>79</v>
       </c>
@@ -4539,7 +4550,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>79</v>
       </c>
@@ -4568,7 +4579,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>79</v>
       </c>
@@ -4597,7 +4608,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>79</v>
       </c>
@@ -4626,7 +4637,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>79</v>
       </c>
@@ -4655,7 +4666,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>79</v>
       </c>
@@ -4684,7 +4695,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>79</v>
       </c>
@@ -4713,7 +4724,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>79</v>
       </c>
@@ -4742,7 +4753,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>79</v>
       </c>
@@ -4768,7 +4779,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>79</v>
       </c>
@@ -4797,7 +4808,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>79</v>
       </c>
@@ -4823,7 +4834,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>79</v>
       </c>
@@ -4855,7 +4866,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>80</v>
       </c>
@@ -4868,7 +4879,7 @@
       <c r="G117" s="9"/>
       <c r="K117" s="8"/>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>80</v>
       </c>
@@ -4879,7 +4890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>80</v>
       </c>
@@ -4890,7 +4901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>36</v>
       </c>
@@ -4919,7 +4930,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>36</v>
       </c>
@@ -4948,7 +4959,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>36</v>
       </c>
@@ -4977,7 +4988,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>36</v>
       </c>
@@ -5006,7 +5017,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>36</v>
       </c>
@@ -5029,7 +5040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>36</v>
       </c>
@@ -5052,7 +5063,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>36</v>
       </c>
@@ -5066,7 +5077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>36</v>
       </c>
@@ -5092,7 +5103,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>36</v>
       </c>
@@ -5109,7 +5120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>31</v>
       </c>
@@ -5138,7 +5149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>31</v>
       </c>
@@ -5173,7 +5184,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>31</v>
       </c>
@@ -5205,7 +5216,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>31</v>
       </c>
@@ -5234,7 +5245,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>31</v>
       </c>
@@ -5266,7 +5277,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>31</v>
       </c>
@@ -5298,7 +5309,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>31</v>
       </c>
@@ -5330,7 +5341,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>37</v>
       </c>
@@ -5341,7 +5352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>35</v>
       </c>
@@ -5355,7 +5366,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>35</v>
       </c>
@@ -5366,7 +5377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>35</v>
       </c>
@@ -5377,7 +5388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>35</v>
       </c>
@@ -5388,7 +5399,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>35</v>
       </c>
@@ -5417,7 +5428,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>35</v>
       </c>
@@ -5446,7 +5457,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>35</v>
       </c>
@@ -5475,7 +5486,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>35</v>
       </c>
@@ -5501,7 +5512,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>35</v>
       </c>
@@ -5530,7 +5541,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>35</v>
       </c>
@@ -5556,7 +5567,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>70</v>
       </c>
@@ -5567,45 +5578,295 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C148" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="D148" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E148" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="F148" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="G148" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A150" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A151" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C151" s="3">
+        <v>1070</v>
+      </c>
+      <c r="D151" s="3">
+        <f>(Table1[[#This Row],[Value 2020]]+Table1[[#This Row],[Value 2030]])/2</f>
+        <v>1045</v>
+      </c>
+      <c r="E151" s="3">
+        <v>1020</v>
+      </c>
+      <c r="F151" s="3">
+        <f>(Table1[[#This Row],[Value 2030]]+Table1[[#This Row],[Value 2050]])/2</f>
+        <v>970</v>
+      </c>
+      <c r="G151" s="3">
+        <v>920</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C153" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="D153" s="3">
+        <f>(Table1[[#This Row],[Value 2020]]+Table1[[#This Row],[Value 2030]])/2</f>
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="E153" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F153" s="3">
+        <f>(Table1[[#This Row],[Value 2030]]+Table1[[#This Row],[Value 2050]])/2</f>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="G153" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A154" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1</v>
+      </c>
+      <c r="D154" s="3">
+        <v>1</v>
+      </c>
+      <c r="E154" s="3">
+        <v>1</v>
+      </c>
+      <c r="F154" s="3">
+        <v>1</v>
+      </c>
+      <c r="G154" s="3">
+        <v>1</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A155" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C155" s="3">
+        <v>1</v>
+      </c>
+      <c r="D155" s="3">
+        <v>1</v>
+      </c>
+      <c r="E155" s="3">
+        <v>1</v>
+      </c>
+      <c r="F155" s="3">
+        <v>1</v>
+      </c>
+      <c r="G155" s="3">
+        <v>1</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C156" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D156" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E156" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="F156" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G156" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -5624,7 +5885,7 @@
           <x14:formula1>
             <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>H187:H1048576 I1:I186</xm:sqref>
+          <xm:sqref>H186:H1048576 I1:I185</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DCFF093-BE81-4C53-B36B-4DFE1729FE77}">
           <x14:formula1>
@@ -5646,10 +5907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B686478B-2667-46C0-A34E-67E3B0146B50}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5767,6 +6028,11 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added efficiencies of methanol storage
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/03_overview_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB826F9-62B9-427C-9AC5-5923765D2015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{4BB826F9-62B9-427C-9AC5-5923765D2015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D05378A6-B898-4675-B733-9EDEBA7BA867}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="261">
   <si>
     <t>Comment</t>
   </si>
@@ -795,6 +795,33 @@
   </si>
   <si>
     <t>for a plant &gt;10MW</t>
+  </si>
+  <si>
+    <t>fix_ratio_out_in_connection_flow</t>
+  </si>
+  <si>
+    <t>fix_ratio_in_out_connection_flow</t>
+  </si>
+  <si>
+    <t>% per 3 days</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijhydene.2020.04.181</t>
+  </si>
+  <si>
+    <t>very small, probably neglectable</t>
+  </si>
+  <si>
+    <t>% per 13 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It takes 13 hours to fully unload a tank of 160 m^3 so for a tank of 450 m^3 around 28.9 hours are needed </t>
+  </si>
+  <si>
+    <t>It takes 13 hours to fully load a tank of 160 m^3 so for a tank of 450 m^3 around 28.9 hours are needed -&gt; convert into %/MWh by using the energy density of methanol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% per 13 hours </t>
   </si>
 </sst>
 </file>
@@ -802,9 +829,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0_)"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -985,15 +1012,15 @@
   </borders>
   <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1002,8 +1029,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1027,7 +1054,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1052,6 +1079,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="36">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{CA87A11B-7565-4B80-9ACA-4E9D38A9573D}"/>
@@ -1145,18 +1173,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K185" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K185" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K187" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K187" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}">
     <filterColumn colId="0">
       <filters>
         <filter val="Electric_Steam_Boiler"/>
+        <filter val="Hydrogen storage"/>
         <filter val="Methanol"/>
+        <filter val="Methanol storage"/>
         <filter val="Methanol_Reactor"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K147">
-    <sortCondition ref="A1:A185"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K149">
+    <sortCondition ref="A1:A187"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6E53C81-05B8-4C0E-A16D-FD48958B7AB9}" name=" " dataDxfId="10"/>
@@ -1472,16 +1502,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
-  <dimension ref="A1:K185"/>
+  <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.90625" style="3" customWidth="1"/>
@@ -1893,11 +1923,11 @@
         <v>72</v>
       </c>
       <c r="C15" s="3">
-        <f>C77</f>
+        <f>C79</f>
         <v>1.35</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ref="D15:G15" si="0">D77</f>
+        <f t="shared" ref="D15:G15" si="0">D79</f>
         <v>1.35</v>
       </c>
       <c r="E15" s="3">
@@ -3138,7 +3168,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>46</v>
       </c>
@@ -3170,7 +3200,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>46</v>
       </c>
@@ -3202,7 +3232,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>46</v>
       </c>
@@ -3231,7 +3261,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>46</v>
       </c>
@@ -3260,7 +3290,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>46</v>
       </c>
@@ -3289,7 +3319,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>46</v>
       </c>
@@ -3346,7 +3376,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>47</v>
       </c>
@@ -3360,7 +3390,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>47</v>
       </c>
@@ -3371,7 +3401,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>47</v>
       </c>
@@ -3382,146 +3412,173 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C65" s="10">
+        <v>9.5999999999999996E-6</v>
+      </c>
+      <c r="D65" s="10">
+        <v>9.5999999999999996E-6</v>
+      </c>
+      <c r="E65" s="10">
+        <v>9.5999999999999996E-6</v>
+      </c>
+      <c r="F65" s="10">
+        <v>9.5999999999999996E-6</v>
+      </c>
+      <c r="G65" s="10">
+        <v>9.5999999999999996E-6</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>97</v>
+        <v>252</v>
+      </c>
+      <c r="C66" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="D66" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="E66" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="F66" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="G66" s="10">
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>98</v>
+        <v>260</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>85</v>
+        <v>47</v>
+      </c>
+      <c r="B67" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="D67" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="E67" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="F67" s="10">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="G67" s="10">
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>93</v>
+        <v>257</v>
       </c>
       <c r="I67" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C68" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="D68" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="E68" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="F68" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="G68" s="3">
-        <v>1.4</v>
+        <v>11</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C69" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="D69" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="E69" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="F69" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="G69" s="3">
-        <v>6.4</v>
+        <v>11</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>220</v>
+        <v>93</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3532,28 +3589,28 @@
         <v>52</v>
       </c>
       <c r="C70" s="3">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="D70" s="3">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="E70" s="3">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="F70" s="3">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="G70" s="3">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>94</v>
@@ -3567,28 +3624,28 @@
         <v>52</v>
       </c>
       <c r="C71" s="3">
-        <v>0.55000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="D71" s="3">
-        <v>0.55000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="E71" s="3">
-        <v>0.55000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="F71" s="3">
-        <v>0.55000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="G71" s="3">
-        <v>0.55000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>94</v>
@@ -3602,28 +3659,28 @@
         <v>52</v>
       </c>
       <c r="C72" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D72" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E72" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F72" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G72" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>94</v>
@@ -3637,28 +3694,28 @@
         <v>52</v>
       </c>
       <c r="C73" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D73" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E73" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F73" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G73" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>94</v>
@@ -3669,28 +3726,31 @@
         <v>34</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C74" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D74" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E74" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F74" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G74" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>92</v>
+        <v>223</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>94</v>
@@ -3701,63 +3761,66 @@
         <v>34</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C75" s="3">
-        <v>39</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D75" s="3">
-        <v>39</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E75" s="3">
-        <v>30</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F75" s="3">
-        <v>30</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G75" s="3">
-        <v>26</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="K75" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>97</v>
+        <v>25</v>
+      </c>
+      <c r="C76" s="3">
+        <v>0</v>
+      </c>
+      <c r="D76" s="3">
+        <v>0</v>
+      </c>
+      <c r="E76" s="3">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3">
+        <v>0</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J76" s="3" t="s">
-        <v>76</v>
+      <c r="K76" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3765,162 +3828,159 @@
         <v>34</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C77" s="3">
-        <v>1.35</v>
+        <v>39</v>
       </c>
       <c r="D77" s="3">
-        <v>1.35</v>
+        <v>39</v>
       </c>
       <c r="E77" s="3">
-        <v>1.0900000000000001</v>
+        <v>30</v>
       </c>
       <c r="F77" s="3">
-        <v>0.96</v>
+        <v>30</v>
       </c>
       <c r="G77" s="3">
-        <v>0.87</v>
+        <v>26</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="I77" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="3">
-        <v>30</v>
-      </c>
-      <c r="D78" s="3">
-        <v>30</v>
-      </c>
-      <c r="E78" s="3">
-        <v>30</v>
-      </c>
-      <c r="F78" s="3">
-        <v>30</v>
-      </c>
-      <c r="G78" s="3">
-        <v>30</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>96</v>
+        <v>75</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K78" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J78" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C79" s="3">
-        <v>50</v>
+        <v>1.35</v>
       </c>
       <c r="D79" s="3">
-        <v>50</v>
+        <v>1.35</v>
       </c>
       <c r="E79" s="3">
-        <v>50</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F79" s="3">
-        <v>50</v>
+        <v>0.96</v>
       </c>
       <c r="G79" s="3">
-        <v>50</v>
+        <v>0.87</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="C80" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D80" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E80" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F80" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G80" s="3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I80" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K80" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>101</v>
+        <v>83</v>
+      </c>
+      <c r="C81" s="3">
+        <v>50</v>
+      </c>
+      <c r="D81" s="3">
+        <v>50</v>
+      </c>
+      <c r="E81" s="3">
+        <v>50</v>
+      </c>
+      <c r="F81" s="3">
+        <v>50</v>
+      </c>
+      <c r="G81" s="3">
+        <v>50</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
@@ -3928,140 +3988,155 @@
         <v>34</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>115</v>
+        <v>84</v>
+      </c>
+      <c r="C82" s="3">
+        <v>50</v>
+      </c>
+      <c r="D82" s="3">
+        <v>50</v>
+      </c>
+      <c r="E82" s="3">
+        <v>50</v>
+      </c>
+      <c r="F82" s="3">
+        <v>50</v>
+      </c>
+      <c r="G82" s="3">
+        <v>50</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I82" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J82" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K82" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>116</v>
+        <v>82</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" s="3">
-        <v>3</v>
-      </c>
-      <c r="D84" s="3">
-        <v>3</v>
-      </c>
-      <c r="E84" s="3">
-        <v>3</v>
-      </c>
-      <c r="F84" s="3">
-        <v>3</v>
-      </c>
-      <c r="G84" s="3">
-        <v>3</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K84" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C85" s="3">
+      <c r="B85" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" s="3">
+        <v>3</v>
+      </c>
+      <c r="D86" s="3">
+        <v>3</v>
+      </c>
+      <c r="E86" s="3">
+        <v>3</v>
+      </c>
+      <c r="F86" s="3">
+        <v>3</v>
+      </c>
+      <c r="G86" s="3">
+        <v>3</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C87" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D87" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E87" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F87" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="G85" s="3">
+      <c r="G87" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="H87" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J85" s="3" t="s">
+      <c r="J87" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K85" s="3" t="s">
+      <c r="K87" s="3" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K86" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C87" s="3">
-        <v>50</v>
-      </c>
-      <c r="E87" s="3">
-        <v>50</v>
-      </c>
-      <c r="G87" s="3">
-        <v>50</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -4069,25 +4144,22 @@
         <v>183</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C88" s="3">
-        <v>10.7</v>
-      </c>
-      <c r="E88" s="3">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="G88" s="3">
-        <v>9.8000000000000007</v>
+        <v>52</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="I88" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="K88" s="3" t="s">
         <v>215</v>
@@ -4098,25 +4170,22 @@
         <v>183</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C89" s="3">
-        <v>7.1</v>
+        <v>50</v>
       </c>
       <c r="E89" s="3">
-        <v>6.8</v>
+        <v>50</v>
       </c>
       <c r="G89" s="3">
-        <v>6.5</v>
+        <v>50</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="K89" s="3" t="s">
         <v>215</v>
@@ -4130,13 +4199,13 @@
         <v>73</v>
       </c>
       <c r="C90" s="3">
-        <v>3</v>
+        <v>10.7</v>
       </c>
       <c r="E90" s="3">
-        <v>2.9</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="G90" s="3">
-        <v>2.7</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>147</v>
@@ -4145,7 +4214,7 @@
         <v>14</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K90" s="3" t="s">
         <v>215</v>
@@ -4159,13 +4228,13 @@
         <v>73</v>
       </c>
       <c r="C91" s="3">
-        <v>1.4</v>
+        <v>7.1</v>
       </c>
       <c r="E91" s="3">
-        <v>1.3</v>
+        <v>6.8</v>
       </c>
       <c r="G91" s="3">
-        <v>1.3</v>
+        <v>6.5</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>147</v>
@@ -4174,7 +4243,7 @@
         <v>14</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K91" s="3" t="s">
         <v>215</v>
@@ -4188,13 +4257,13 @@
         <v>73</v>
       </c>
       <c r="C92" s="3">
-        <v>0.7</v>
+        <v>3</v>
       </c>
       <c r="E92" s="3">
-        <v>0.7</v>
+        <v>2.9</v>
       </c>
       <c r="G92" s="3">
-        <v>0.7</v>
+        <v>2.7</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>147</v>
@@ -4203,7 +4272,7 @@
         <v>14</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K92" s="3" t="s">
         <v>215</v>
@@ -4217,13 +4286,13 @@
         <v>73</v>
       </c>
       <c r="C93" s="3">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="E93" s="3">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="G93" s="3">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>147</v>
@@ -4232,7 +4301,7 @@
         <v>14</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="K93" s="3" t="s">
         <v>215</v>
@@ -4246,13 +4315,13 @@
         <v>73</v>
       </c>
       <c r="C94" s="3">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="E94" s="3">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="G94" s="3">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>147</v>
@@ -4261,7 +4330,7 @@
         <v>14</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K94" s="3" t="s">
         <v>215</v>
@@ -4275,13 +4344,13 @@
         <v>73</v>
       </c>
       <c r="C95" s="3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E95" s="3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G95" s="3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>147</v>
@@ -4290,7 +4359,7 @@
         <v>14</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="K95" s="3" t="s">
         <v>215</v>
@@ -4301,22 +4370,25 @@
         <v>183</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C96" s="3">
-        <v>106</v>
+        <v>0.3</v>
       </c>
       <c r="E96" s="3">
-        <v>106</v>
+        <v>0.2</v>
       </c>
       <c r="G96" s="3">
-        <v>106</v>
+        <v>0.2</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="I96" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="K96" s="3" t="s">
         <v>215</v>
@@ -4327,22 +4399,25 @@
         <v>183</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C97" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E97" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G97" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="I97" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="K97" s="3" t="s">
         <v>215</v>
@@ -4350,45 +4425,54 @@
     </row>
     <row r="98" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>136</v>
+        <v>24</v>
       </c>
       <c r="C98" s="3">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="E98" s="3">
-        <v>2</v>
-      </c>
-      <c r="F98" s="3">
-        <v>1.5</v>
+        <v>106</v>
       </c>
       <c r="G98" s="3">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="I98" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K98" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="C99" s="3">
+        <v>0</v>
+      </c>
+      <c r="E99" s="3">
+        <v>0</v>
+      </c>
+      <c r="G99" s="3">
+        <v>0</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J99" s="3" t="s">
-        <v>55</v>
+      <c r="K99" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -4396,57 +4480,42 @@
         <v>79</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>164</v>
+        <v>136</v>
+      </c>
+      <c r="C100" s="3">
+        <v>3</v>
+      </c>
+      <c r="E100" s="3">
+        <v>2</v>
+      </c>
+      <c r="F100" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G100" s="3">
+        <v>1</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J100" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="K100" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="I101" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="K101" s="3" t="s">
-        <v>215</v>
+        <v>55</v>
       </c>
     </row>
     <row r="102" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -4457,13 +4526,13 @@
         <v>52</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>149</v>
@@ -4472,7 +4541,7 @@
         <v>14</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K102" s="3" t="s">
         <v>215</v>
@@ -4486,13 +4555,13 @@
         <v>52</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>149</v>
@@ -4501,7 +4570,7 @@
         <v>14</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K103" s="3" t="s">
         <v>215</v>
@@ -4515,13 +4584,13 @@
         <v>52</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>149</v>
@@ -4530,7 +4599,7 @@
         <v>14</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K104" s="3" t="s">
         <v>215</v>
@@ -4544,13 +4613,13 @@
         <v>52</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>149</v>
@@ -4559,7 +4628,7 @@
         <v>14</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K105" s="3" t="s">
         <v>215</v>
@@ -4573,13 +4642,13 @@
         <v>52</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G106" s="3">
-        <v>1.3</v>
+        <v>161</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>149</v>
@@ -4588,7 +4657,7 @@
         <v>14</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K106" s="3" t="s">
         <v>215</v>
@@ -4599,25 +4668,25 @@
         <v>79</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I107" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K107" s="3" t="s">
         <v>215</v>
@@ -4628,25 +4697,25 @@
         <v>79</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>146</v>
+        <v>163</v>
+      </c>
+      <c r="G108" s="3">
+        <v>1.3</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I108" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="K108" s="3" t="s">
         <v>215</v>
@@ -4660,13 +4729,13 @@
         <v>73</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G109" s="3">
-        <v>1.1000000000000001</v>
+        <v>143</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>147</v>
@@ -4675,7 +4744,7 @@
         <v>14</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="K109" s="3" t="s">
         <v>215</v>
@@ -4689,13 +4758,13 @@
         <v>73</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E110" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="G110" s="3">
-        <v>0.7</v>
+        <v>140</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>147</v>
@@ -4704,7 +4773,7 @@
         <v>14</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K110" s="3" t="s">
         <v>215</v>
@@ -4717,14 +4786,14 @@
       <c r="B111" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C111" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="E111" s="3">
-        <v>0.4</v>
+      <c r="C111" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="G111" s="3">
-        <v>0.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>147</v>
@@ -4733,7 +4802,7 @@
         <v>14</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K111" s="3" t="s">
         <v>215</v>
@@ -4746,14 +4815,14 @@
       <c r="B112" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C112" s="3">
-        <v>0.2</v>
+      <c r="C112" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="E112" s="3">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="G112" s="3">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>147</v>
@@ -4762,7 +4831,7 @@
         <v>14</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K112" s="3" t="s">
         <v>215</v>
@@ -4773,22 +4842,25 @@
         <v>79</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C113" s="3">
-        <v>50</v>
+        <v>0.4</v>
       </c>
       <c r="E113" s="3">
-        <v>50</v>
+        <v>0.4</v>
       </c>
       <c r="G113" s="3">
-        <v>50</v>
+        <v>0.4</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="I113" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="K113" s="3" t="s">
         <v>215</v>
@@ -4799,25 +4871,25 @@
         <v>79</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C114" s="3">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E114" s="3">
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
       <c r="G114" s="3">
         <v>0.2</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="I114" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K114" s="3" t="s">
         <v>215</v>
@@ -4828,19 +4900,19 @@
         <v>79</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C115" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E115" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G115" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>196</v>
+        <v>96</v>
       </c>
       <c r="I115" s="3" t="s">
         <v>14</v>
@@ -4854,55 +4926,86 @@
         <v>79</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E116" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="G116" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" s="3">
+        <v>0</v>
+      </c>
+      <c r="E117" s="3">
+        <v>0</v>
+      </c>
+      <c r="G117" s="3">
+        <v>0</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C116" s="9">
+      <c r="C118" s="9">
         <v>0.88</v>
       </c>
-      <c r="E116" s="9">
+      <c r="E118" s="9">
         <v>0.89</v>
       </c>
-      <c r="F116" s="9">
+      <c r="F118" s="9">
         <v>0.9</v>
       </c>
-      <c r="G116" s="9">
+      <c r="G118" s="9">
         <v>0.9</v>
       </c>
-      <c r="H116" s="3" t="s">
+      <c r="H118" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="I116" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J116" s="3" t="s">
+      <c r="I118" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J118" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="K116" s="8" t="s">
+      <c r="K118" s="8" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C117" s="9"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="9"/>
-      <c r="G117" s="9"/>
-      <c r="K117" s="8"/>
-    </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -4910,68 +5013,34 @@
         <v>80</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="K119" s="8"/>
+    </row>
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C120" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="G120" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="I120" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J120" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="K120" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="G121" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H121" s="3" t="s">
-        <v>197</v>
+        <v>74</v>
       </c>
       <c r="I121" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J121" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K121" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -4982,13 +5051,13 @@
         <v>73</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>197</v>
@@ -4997,7 +5066,7 @@
         <v>14</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K122" s="3" t="s">
         <v>215</v>
@@ -5011,13 +5080,13 @@
         <v>73</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H123" s="3" t="s">
         <v>197</v>
@@ -5026,56 +5095,68 @@
         <v>14</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K123" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C124" s="3">
-        <v>40</v>
-      </c>
-      <c r="E124" s="3">
-        <v>40</v>
-      </c>
-      <c r="G124" s="3">
-        <v>40</v>
+        <v>73</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="I124" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="J124" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C125" s="3">
-        <v>3398</v>
-      </c>
-      <c r="E125" s="3">
-        <v>3562</v>
-      </c>
-      <c r="G125" s="3">
-        <v>3735</v>
+        <v>73</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I125" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="K125" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5083,13 +5164,22 @@
         <v>36</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>50</v>
+        <v>74</v>
+      </c>
+      <c r="C126" s="3">
+        <v>40</v>
+      </c>
+      <c r="E126" s="3">
+        <v>40</v>
+      </c>
+      <c r="G126" s="3">
+        <v>40</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J126" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5097,138 +5187,108 @@
         <v>36</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>208</v>
+        <v>24</v>
+      </c>
+      <c r="C127" s="3">
+        <v>3398</v>
+      </c>
+      <c r="E127" s="3">
+        <v>3562</v>
+      </c>
+      <c r="G127" s="3">
+        <v>3735</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="I127" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J127" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J128" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K128" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H129" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I129" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="I130" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J130" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K130" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C131" s="3">
-        <v>0</v>
-      </c>
-      <c r="D131" s="3">
-        <v>0</v>
-      </c>
-      <c r="E131" s="3">
-        <v>0</v>
-      </c>
-      <c r="F131" s="3">
-        <v>0</v>
-      </c>
-      <c r="G131" s="3">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="I131" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="K131" s="3" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="132" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -5236,7 +5296,7 @@
         <v>31</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>97</v>
@@ -5253,11 +5313,17 @@
       <c r="G132" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="H132" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="I132" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>76</v>
+        <v>57</v>
+      </c>
+      <c r="K132" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -5265,25 +5331,25 @@
         <v>31</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="C133" s="3">
-        <v>0.56000000000000005</v>
+        <v>0</v>
       </c>
       <c r="D133" s="3">
-        <v>0.56000000000000005</v>
+        <v>0</v>
       </c>
       <c r="E133" s="3">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="F133" s="3">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="G133" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>226</v>
+        <v>109</v>
       </c>
       <c r="I133" s="3" t="s">
         <v>14</v>
@@ -5292,36 +5358,33 @@
         <v>228</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C134" s="3">
-        <v>35</v>
-      </c>
-      <c r="D134" s="3">
-        <v>35</v>
-      </c>
-      <c r="E134" s="3">
-        <v>40</v>
-      </c>
-      <c r="F134" s="3">
-        <v>40</v>
-      </c>
-      <c r="G134" s="3">
-        <v>40</v>
-      </c>
-      <c r="H134" s="3" t="s">
-        <v>96</v>
+        <v>75</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="I134" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K134" s="3" t="s">
-        <v>228</v>
+      <c r="J134" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="135" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -5329,25 +5392,25 @@
         <v>31</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="C135" s="3">
-        <v>11300</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D135" s="3">
-        <v>11300</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E135" s="3">
-        <v>9500</v>
+        <v>0.38</v>
       </c>
       <c r="F135" s="3">
-        <v>8100</v>
+        <v>0.32</v>
       </c>
       <c r="G135" s="3">
-        <v>7400</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I135" s="3" t="s">
         <v>14</v>
@@ -5356,40 +5419,79 @@
         <v>228</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="C136" s="3">
+        <v>35</v>
+      </c>
+      <c r="D136" s="3">
+        <v>35</v>
+      </c>
+      <c r="E136" s="3">
+        <v>40</v>
+      </c>
+      <c r="F136" s="3">
+        <v>40</v>
+      </c>
+      <c r="G136" s="3">
+        <v>40</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="I136" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K136" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="C137" s="3">
+        <v>11300</v>
+      </c>
+      <c r="D137" s="3">
+        <v>11300</v>
+      </c>
+      <c r="E137" s="3">
+        <v>9500</v>
+      </c>
+      <c r="F137" s="3">
+        <v>8100</v>
+      </c>
+      <c r="G137" s="3">
+        <v>7400</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="I137" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J137" s="3" t="s">
-        <v>51</v>
+      <c r="K137" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5397,10 +5499,13 @@
         <v>35</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J139" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5408,68 +5513,32 @@
         <v>35</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J140" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="E141" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="G141" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="H141" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I141" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="K141" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E142" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="G142" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="H142" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I142" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K142" s="3" t="s">
-        <v>215</v>
+        <v>64</v>
       </c>
     </row>
     <row r="143" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -5480,13 +5549,13 @@
         <v>73</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H143" s="3" t="s">
         <v>197</v>
@@ -5495,7 +5564,7 @@
         <v>14</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K143" s="3" t="s">
         <v>215</v>
@@ -5506,22 +5575,25 @@
         <v>35</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C144" s="3">
-        <v>40</v>
-      </c>
-      <c r="E144" s="3">
-        <v>40</v>
-      </c>
-      <c r="G144" s="3">
-        <v>40</v>
+        <v>73</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G144" s="6" t="s">
+        <v>210</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="I144" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="K144" s="3" t="s">
         <v>215</v>
@@ -5532,25 +5604,25 @@
         <v>35</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E145" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="G145" s="7" t="s">
-        <v>212</v>
+        <v>73</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G145" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="I145" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="K145" s="3" t="s">
         <v>215</v>
@@ -5561,19 +5633,19 @@
         <v>35</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C146" s="3">
-        <v>1.595</v>
+        <v>40</v>
       </c>
       <c r="E146" s="3">
-        <v>1.595</v>
+        <v>40</v>
       </c>
       <c r="G146" s="3">
-        <v>1.595</v>
+        <v>40</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="I146" s="3" t="s">
         <v>14</v>
@@ -5582,142 +5654,131 @@
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C148" s="3">
+        <v>1.595</v>
+      </c>
+      <c r="E148" s="3">
+        <v>1.595</v>
+      </c>
+      <c r="G148" s="3">
+        <v>1.595</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B149" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I147" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A148" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C148" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="D148" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="E148" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="F148" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="G148" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="H148" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J148" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="K148" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A149" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G149" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H149" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="I149" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K149" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E150" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F150" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="C150" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="D150" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E150" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="F150" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="G150" s="3">
+        <v>0.99</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="K150" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C151" s="3">
-        <v>1070</v>
-      </c>
-      <c r="D151" s="3">
-        <f>(Table1[[#This Row],[Value 2020]]+Table1[[#This Row],[Value 2030]])/2</f>
-        <v>1045</v>
-      </c>
-      <c r="E151" s="3">
-        <v>1020</v>
-      </c>
-      <c r="F151" s="3">
-        <f>(Table1[[#This Row],[Value 2030]]+Table1[[#This Row],[Value 2050]])/2</f>
-        <v>970</v>
-      </c>
-      <c r="G151" s="3">
-        <v>920</v>
+        <v>11</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>249</v>
+        <v>98</v>
       </c>
       <c r="I151" s="3" t="s">
         <v>14</v>
@@ -5726,33 +5787,33 @@
         <v>228</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J152" s="3" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
       <c r="K152" s="3" t="s">
         <v>228</v>
@@ -5763,33 +5824,30 @@
         <v>245</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C153" s="3">
-        <v>0.15</v>
+        <v>1070</v>
       </c>
       <c r="D153" s="3">
         <f>(Table1[[#This Row],[Value 2020]]+Table1[[#This Row],[Value 2030]])/2</f>
-        <v>0.14500000000000002</v>
+        <v>1045</v>
       </c>
       <c r="E153" s="3">
-        <v>0.14000000000000001</v>
+        <v>1020</v>
       </c>
       <c r="F153" s="3">
         <f>(Table1[[#This Row],[Value 2030]]+Table1[[#This Row],[Value 2050]])/2</f>
-        <v>0.13500000000000001</v>
+        <v>970</v>
       </c>
       <c r="G153" s="3">
-        <v>0.13</v>
+        <v>920</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I153" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="J153" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="K153" s="3" t="s">
         <v>228</v>
@@ -5800,25 +5858,28 @@
         <v>245</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C154" s="3">
-        <v>1</v>
-      </c>
-      <c r="D154" s="3">
-        <v>1</v>
-      </c>
-      <c r="E154" s="3">
-        <v>1</v>
-      </c>
-      <c r="F154" s="3">
-        <v>1</v>
-      </c>
-      <c r="G154" s="3">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="I154" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="K154" s="3" t="s">
         <v>228</v>
@@ -5829,25 +5890,33 @@
         <v>245</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C155" s="3">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="D155" s="3">
-        <v>1</v>
+        <f>(Table1[[#This Row],[Value 2020]]+Table1[[#This Row],[Value 2030]])/2</f>
+        <v>0.14500000000000002</v>
       </c>
       <c r="E155" s="3">
-        <v>1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F155" s="3">
-        <v>1</v>
+        <f>(Table1[[#This Row],[Value 2030]]+Table1[[#This Row],[Value 2050]])/2</f>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G155" s="3">
-        <v>1</v>
+        <v>0.13</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="I155" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="K155" s="3" t="s">
         <v>228</v>
@@ -5858,25 +5927,22 @@
         <v>245</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C156" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="D156" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="E156" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="F156" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="G156" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="H156" s="3" t="s">
-        <v>248</v>
+        <v>83</v>
+      </c>
+      <c r="C156" s="3">
+        <v>1</v>
+      </c>
+      <c r="D156" s="3">
+        <v>1</v>
+      </c>
+      <c r="E156" s="3">
+        <v>1</v>
+      </c>
+      <c r="F156" s="3">
+        <v>1</v>
+      </c>
+      <c r="G156" s="3">
+        <v>1</v>
       </c>
       <c r="I156" s="3" t="s">
         <v>14</v>
@@ -5885,8 +5951,67 @@
         <v>228</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="157" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A157" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C157" s="3">
+        <v>1</v>
+      </c>
+      <c r="D157" s="3">
+        <v>1</v>
+      </c>
+      <c r="E157" s="3">
+        <v>1</v>
+      </c>
+      <c r="F157" s="3">
+        <v>1</v>
+      </c>
+      <c r="G157" s="3">
+        <v>1</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A158" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C158" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D158" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E158" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="F158" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G158" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
     <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="161" hidden="1" x14ac:dyDescent="0.35"/>
@@ -5914,11 +6039,13 @@
     <row r="183" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="184" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="185" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" display="https://cdn.website-editor.net/s/b1c3966c02424fcdb65f54c67900e60d/files/uploaded/CO2-Verdampfer-CL.pdf?Expires=1714516055&amp;Signature=m06pYyARv0DK17fQ8SPW8vwf9jnMfU4P1ain0XsTdf5IC0YISOgOSZihUu3pNmFjKZBAf2Cyc6Dugk5rrrRTrC3LWGX3wT4hRWqqa1u5kyZiKcGOp0V~EjlTKlgDr1QLcsIT7wCPo1IWSp-XVCuaVkRF86EZ3cGv2z3X9L5SWC~O23VX6iWRnfDenuvCfdcKCDfIuQP9AEtd-qzdjIBRdR0ByJcG5pBolT58m--TIeugDUruhTfMuKrCMhVrmWzo0Gk63KPF7ZTlVJeM-Xue7Sz0nm7BgrQlxLdO4whUGMoTmum05h4-REKvtnpOhDrx~vGOVMTk7zcVwvel~KBeww__&amp;Key-Pair-Id=K2NXBXLF010TJW" xr:uid="{DBDAD553-33AA-4DBF-ACAE-0382B8D931C1}"/>
-    <hyperlink ref="K116" r:id="rId2" xr:uid="{C15DCB95-DC96-4E12-BC5C-638AF89A1D76}"/>
+    <hyperlink ref="K118" r:id="rId2" xr:uid="{C15DCB95-DC96-4E12-BC5C-638AF89A1D76}"/>
     <hyperlink ref="K57" r:id="rId3" xr:uid="{52B939ED-8287-4285-896D-B0F6FE3A0772}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5932,7 +6059,7 @@
           <x14:formula1>
             <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>H186:H1048576 I1:I185</xm:sqref>
+          <xm:sqref>H188:H1048576 I1:I187</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DCFF093-BE81-4C53-B36B-4DFE1729FE77}">
           <x14:formula1>
@@ -5956,7 +6083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B686478B-2667-46C0-A34E-67E3B0146B50}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -6089,9 +6216,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A04CB00-B233-4C8F-9598-9E4FA54AC391}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -6264,7 +6391,12 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated methanol storage efficiencies
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/03_overview_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{4BB826F9-62B9-427C-9AC5-5923765D2015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D05378A6-B898-4675-B733-9EDEBA7BA867}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{4BB826F9-62B9-427C-9AC5-5923765D2015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23D0388D-CD08-4286-9284-D9FE1B988BCB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
@@ -815,13 +815,13 @@
     <t>% per 13 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">It takes 13 hours to fully unload a tank of 160 m^3 so for a tank of 450 m^3 around 28.9 hours are needed </t>
-  </si>
-  <si>
-    <t>It takes 13 hours to fully load a tank of 160 m^3 so for a tank of 450 m^3 around 28.9 hours are needed -&gt; convert into %/MWh by using the energy density of methanol</t>
-  </si>
-  <si>
     <t xml:space="preserve">% per 13 hours </t>
+  </si>
+  <si>
+    <t>It takes 13 hours to fully load a tank of 160 m^3 so for a tank of 480 m^3 around 39 hours are needed -&gt; convert into %/MWh by using the energy density of methanol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It takes 13 hours to fully unload a tank of 160 m^3 so for a tank of 480 m^3 around 39 hours are needed </t>
   </si>
 </sst>
 </file>
@@ -1172,6 +1172,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}" name="Table1" displayName="Table1" ref="A1:K187" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K187" xr:uid="{4F9B01EA-EBEA-4741-AB35-4EF8891F463E}">
@@ -1504,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
   <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="H55" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3470,7 +3474,7 @@
         <v>1.6000000000000001E-4</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>14</v>
@@ -3511,7 +3515,7 @@
         <v>14</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="K67" s="3" t="s">
         <v>255</v>

</xml_diff>

<commit_message>
update investment cost overview data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605ABF67-A6D6-43E3-B6F9-35CE94DF2CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884F7B86-869C-4F50-8595-B65790503BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="266">
   <si>
     <t>Comment</t>
   </si>
@@ -831,6 +831,12 @@
   </si>
   <si>
     <t>Euro/kg Fuel</t>
+  </si>
+  <si>
+    <t>Euro/MW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assumption, based on public cost information of vaporizers. The problem is that there is no database with this data. We used public offers for vaporizers to calculate the estimated cost.  </t>
   </si>
 </sst>
 </file>
@@ -1504,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
   <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1739,30 +1745,36 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>97</v>
+      <c r="C8" s="3">
+        <v>500000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>500000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>500000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>500000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>500000</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -3241,6 +3253,10 @@
       </c>
       <c r="C56" s="3">
         <v>0.121</v>
+      </c>
+      <c r="D56" s="3">
+        <f>Table1[[#This Row],[Value 2020]]+Table1[[#This Row],[Value 2030]]/2</f>
+        <v>0.17049999999999998</v>
       </c>
       <c r="E56" s="3">
         <v>9.9000000000000005E-2</v>

</xml_diff>

<commit_message>
update output prepared files
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\03_overview_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C10C08-5B06-4DA2-8D68-E33D7560A03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C68D226-809F-4553-B1C4-90F86082B6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
+    <workbookView xWindow="-3330" yWindow="-20460" windowWidth="28800" windowHeight="15225" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
   <dimension ref="A1:K169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B164" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added investment costs for methane production
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
+++ b/Spine_Projects/01_input_data/03_overview_input/data_needed_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/03_overview_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="13_ncr:1_{50C10C08-5B06-4DA2-8D68-E33D7560A03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4772392C-AC60-46C6-AE87-4910F633F3CD}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="13_ncr:1_{50C10C08-5B06-4DA2-8D68-E33D7560A03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78FC242F-0D73-486E-B255-F07D710681E6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D6FAD9C-9038-4702-924D-B7AFA621FEAD}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="305">
   <si>
     <t>Comment</t>
   </si>
@@ -973,6 +973,21 @@
   </si>
   <si>
     <t>not given in catalogue</t>
+  </si>
+  <si>
+    <t>marked as N.A. in sheet</t>
+  </si>
+  <si>
+    <t>Digester</t>
+  </si>
+  <si>
+    <t>Methane_Plant</t>
+  </si>
+  <si>
+    <t>CO2_Remover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value in datasheet for Methane Plant, Digester and Co2 Remover combined </t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1276,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1678,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55010A2-A2F7-4693-8A24-9D54587F1957}">
   <dimension ref="A1:K247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D211" sqref="D211"/>
+    <sheetView tabSelected="1" topLeftCell="I208" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K218" sqref="K218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6585,6 +6600,24 @@
       <c r="B170" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C170" s="3">
+        <v>30</v>
+      </c>
+      <c r="E170" s="3">
+        <v>30</v>
+      </c>
+      <c r="F170" s="3">
+        <v>30</v>
+      </c>
+      <c r="G170" s="3">
+        <v>30</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="J170" s="3" t="s">
         <v>299</v>
       </c>
@@ -6748,6 +6781,9 @@
       <c r="B178" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="J178" s="3" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
@@ -6782,6 +6818,27 @@
       <c r="A180" s="3" t="s">
         <v>279</v>
       </c>
+      <c r="B180" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C180" s="3">
+        <v>1</v>
+      </c>
+      <c r="E180" s="3">
+        <v>1</v>
+      </c>
+      <c r="F180" s="3">
+        <v>1</v>
+      </c>
+      <c r="G180" s="3">
+        <v>1</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="J180" s="3" t="s">
         <v>282</v>
       </c>
@@ -6936,6 +6993,9 @@
       <c r="G185" s="3">
         <v>0</v>
       </c>
+      <c r="H185" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="I185" s="3" t="s">
         <v>14</v>
       </c>
@@ -6950,6 +7010,27 @@
       <c r="A186" s="3" t="s">
         <v>281</v>
       </c>
+      <c r="B186" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C186" s="3">
+        <v>1</v>
+      </c>
+      <c r="E186" s="3">
+        <v>1</v>
+      </c>
+      <c r="F186" s="3">
+        <v>1</v>
+      </c>
+      <c r="G186" s="3">
+        <v>1</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I186" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="J186" s="3" t="s">
         <v>282</v>
       </c>
@@ -7647,10 +7728,113 @@
         <v>297</v>
       </c>
     </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A211" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C211" s="3">
+        <v>9600000</v>
+      </c>
+      <c r="D211" s="3">
+        <v>2100000</v>
+      </c>
+      <c r="E211" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="F211" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="G211" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="H211" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J211" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="K211" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A212" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C212" s="3">
+        <v>1</v>
+      </c>
+      <c r="D212" s="3">
+        <v>1</v>
+      </c>
+      <c r="E212" s="3">
+        <v>1</v>
+      </c>
+      <c r="F212" s="3">
+        <v>1</v>
+      </c>
+      <c r="G212" s="3">
+        <v>1</v>
+      </c>
+      <c r="H212" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J212" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="K212" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A213" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C213" s="3">
+        <v>1</v>
+      </c>
+      <c r="D213" s="3">
+        <v>1</v>
+      </c>
+      <c r="E213" s="3">
+        <v>1</v>
+      </c>
+      <c r="F213" s="3">
+        <v>1</v>
+      </c>
+      <c r="G213" s="3">
+        <v>1</v>
+      </c>
+      <c r="H213" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J213" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="K213" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A247" s="12" t="s">
-        <v>288</v>
-      </c>
+      <c r="A247" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -7676,7 +7860,7 @@
           <x14:formula1>
             <xm:f>'Variable Types'!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>H210:H1048576 I1:I245</xm:sqref>
+          <xm:sqref>H214:H1048576 H210 I1:I245</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7911B029-FECC-467E-9742-40BD9EB9AF02}">
           <x14:formula1>
@@ -7698,10 +7882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B686478B-2667-46C0-A34E-67E3B0146B50}">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7889,6 +8073,26 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>